<commit_message>
completed the points 3.5; 3.6; 4; 5.
</commit_message>
<xml_diff>
--- a/Create file/test3.xlsx
+++ b/Create file/test3.xlsx
@@ -932,6 +932,23 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1697543492003</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000046279127-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="28">
       <c r="C28" t="inlineStr">
         <is>
@@ -1034,6 +1051,40 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1697725508396</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000046395600-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1697725689512</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000046395867-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="36">
       <c r="C36" t="inlineStr">
         <is>
@@ -1136,6 +1187,23 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>1697804597693</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000046443231-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="43">
       <c r="C43" t="inlineStr">
         <is>
@@ -1357,6 +1425,23 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>1698423620183</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000046791276-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="57">
       <c r="C57" t="inlineStr">
         <is>
@@ -1680,6 +1765,23 @@
         </is>
       </c>
     </row>
+    <row r="76">
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>1699084236528</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047129451-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="77">
       <c r="C77" t="inlineStr">
         <is>
@@ -2309,6 +2411,23 @@
         </is>
       </c>
     </row>
+    <row r="114">
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>1699097481637</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047144108-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="115">
       <c r="C115" t="inlineStr">
         <is>
@@ -3635,6 +3754,23 @@
         </is>
       </c>
     </row>
+    <row r="193">
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>1699339658202</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047253256-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="194">
       <c r="C194" t="inlineStr">
         <is>
@@ -5250,6 +5386,23 @@
         </is>
       </c>
     </row>
+    <row r="289">
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>1699433106967</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047311944-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="290">
       <c r="C290" t="inlineStr">
         <is>
@@ -6321,6 +6474,23 @@
         </is>
       </c>
     </row>
+    <row r="353">
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>1699529197472</t>
+        </is>
+      </c>
+      <c r="G353" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H353" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047375065-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="354">
       <c r="C354" t="inlineStr">
         <is>
@@ -6389,6 +6559,23 @@
         </is>
       </c>
     </row>
+    <row r="358">
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>1699531827062</t>
+        </is>
+      </c>
+      <c r="G358" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H358" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047378210-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="359">
       <c r="C359" t="inlineStr">
         <is>
@@ -6984,6 +7171,23 @@
         </is>
       </c>
     </row>
+    <row r="394">
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>1699696880786</t>
+        </is>
+      </c>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H394" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047469059-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="395">
       <c r="C395" t="inlineStr">
         <is>
@@ -7018,6 +7222,23 @@
         </is>
       </c>
     </row>
+    <row r="397">
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>1699679800863</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H397" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047455831-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="398">
       <c r="C398" t="inlineStr">
         <is>
@@ -7188,6 +7409,23 @@
         </is>
       </c>
     </row>
+    <row r="408">
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>1699602032226</t>
+        </is>
+      </c>
+      <c r="G408" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H408" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047413410-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="409">
       <c r="C409" t="inlineStr">
         <is>
@@ -7834,6 +8072,23 @@
         </is>
       </c>
     </row>
+    <row r="447">
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>1699621580839</t>
+        </is>
+      </c>
+      <c r="G447" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H447" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047436146-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="448">
       <c r="C448" t="inlineStr">
         <is>
@@ -7885,6 +8140,23 @@
         </is>
       </c>
     </row>
+    <row r="451">
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>1699621753244</t>
+        </is>
+      </c>
+      <c r="G451" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H451" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047436254-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="452">
       <c r="C452" t="inlineStr">
         <is>
@@ -7902,6 +8174,23 @@
         </is>
       </c>
     </row>
+    <row r="453">
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>1699621721623</t>
+        </is>
+      </c>
+      <c r="G453" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H453" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047436305-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="454">
       <c r="C454" t="inlineStr">
         <is>
@@ -7919,6 +8208,40 @@
         </is>
       </c>
     </row>
+    <row r="455">
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>1699622068552</t>
+        </is>
+      </c>
+      <c r="G455" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H455" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047436560-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>1699621890692</t>
+        </is>
+      </c>
+      <c r="G456" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H456" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047436586-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="457">
       <c r="C457" t="inlineStr">
         <is>
@@ -7936,6 +8259,74 @@
         </is>
       </c>
     </row>
+    <row r="458">
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>1699622465935</t>
+        </is>
+      </c>
+      <c r="G458" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H458" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047436646-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>1699622396153</t>
+        </is>
+      </c>
+      <c r="G459" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H459" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047436652-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>1699621580189</t>
+        </is>
+      </c>
+      <c r="G460" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H460" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047436659-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>1699622420444</t>
+        </is>
+      </c>
+      <c r="G461" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H461" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047436697-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="462">
       <c r="C462" t="inlineStr">
         <is>
@@ -7970,6 +8361,57 @@
         </is>
       </c>
     </row>
+    <row r="464">
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>1699622846987</t>
+        </is>
+      </c>
+      <c r="G464" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H464" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047436986-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>1699622328764</t>
+        </is>
+      </c>
+      <c r="G465" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H465" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047437024-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>1699622501047</t>
+        </is>
+      </c>
+      <c r="G466" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H466" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047437150-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="467">
       <c r="C467" t="inlineStr">
         <is>
@@ -8225,6 +8667,23 @@
         </is>
       </c>
     </row>
+    <row r="482">
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>1699624991057</t>
+        </is>
+      </c>
+      <c r="G482" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H482" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047438966-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="483">
       <c r="C483" t="inlineStr">
         <is>
@@ -8259,6 +8718,57 @@
         </is>
       </c>
     </row>
+    <row r="485">
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>1699624774727</t>
+        </is>
+      </c>
+      <c r="G485" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H485" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047439171-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>1699625607453</t>
+        </is>
+      </c>
+      <c r="G486" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H486" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047439332-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>1699625957321</t>
+        </is>
+      </c>
+      <c r="G487" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H487" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047439553-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="488">
       <c r="C488" t="inlineStr">
         <is>
@@ -8310,6 +8820,23 @@
         </is>
       </c>
     </row>
+    <row r="491">
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>1699628089667</t>
+        </is>
+      </c>
+      <c r="G491" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H491" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047441042-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="492">
       <c r="C492" t="inlineStr">
         <is>
@@ -8395,6 +8922,23 @@
         </is>
       </c>
     </row>
+    <row r="497">
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>1699629736284</t>
+        </is>
+      </c>
+      <c r="G497" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H497" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047442622-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="498">
       <c r="C498" t="inlineStr">
         <is>
@@ -8412,6 +8956,23 @@
         </is>
       </c>
     </row>
+    <row r="499">
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>1699630818045</t>
+        </is>
+      </c>
+      <c r="G499" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H499" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047443022-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="500">
       <c r="C500" t="inlineStr">
         <is>
@@ -8599,6 +9160,40 @@
         </is>
       </c>
     </row>
+    <row r="511">
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>1699636868271</t>
+        </is>
+      </c>
+      <c r="G511" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H511" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047446357-C1 has dropped the video KYC. Ask the client to complete it by using this link http://www.axisbank.com/vkyc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>1699639421197</t>
+        </is>
+      </c>
+      <c r="G512" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H512" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047447576-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="513">
       <c r="C513" t="inlineStr">
         <is>
@@ -8684,6 +9279,23 @@
         </is>
       </c>
     </row>
+    <row r="518">
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>1699646652041</t>
+        </is>
+      </c>
+      <c r="G518" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H518" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047449473-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="519">
       <c r="C519" t="inlineStr">
         <is>
@@ -8752,6 +9364,23 @@
         </is>
       </c>
     </row>
+    <row r="523">
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>1699677144147</t>
+        </is>
+      </c>
+      <c r="G523" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H523" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047454062-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="524">
       <c r="C524" t="inlineStr">
         <is>
@@ -8769,6 +9398,23 @@
         </is>
       </c>
     </row>
+    <row r="525">
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>1699677888648</t>
+        </is>
+      </c>
+      <c r="G525" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H525" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047454482-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="526">
       <c r="C526" t="inlineStr">
         <is>
@@ -9755,6 +10401,23 @@
         </is>
       </c>
     </row>
+    <row r="584">
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>1699783259192</t>
+        </is>
+      </c>
+      <c r="G584" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H584" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047496863-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="585">
       <c r="C585" t="inlineStr">
         <is>
@@ -10231,6 +10894,23 @@
         </is>
       </c>
     </row>
+    <row r="613">
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>1699952409623</t>
+        </is>
+      </c>
+      <c r="G613" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H613" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047562263-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="614">
       <c r="C614" t="inlineStr">
         <is>
@@ -10486,6 +11166,23 @@
         </is>
       </c>
     </row>
+    <row r="629">
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>1699980332669</t>
+        </is>
+      </c>
+      <c r="G629" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H629" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047582122-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="630">
       <c r="C630" t="inlineStr">
         <is>
@@ -10503,6 +11200,23 @@
         </is>
       </c>
     </row>
+    <row r="631">
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>1699980366608</t>
+        </is>
+      </c>
+      <c r="G631" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H631" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047582254-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="632">
       <c r="C632" t="inlineStr">
         <is>
@@ -10554,6 +11268,23 @@
         </is>
       </c>
     </row>
+    <row r="635">
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>1699980979759</t>
+        </is>
+      </c>
+      <c r="G635" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H635" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047582541-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="636">
       <c r="C636" t="inlineStr">
         <is>
@@ -10571,6 +11302,23 @@
         </is>
       </c>
     </row>
+    <row r="637">
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>1699982544143</t>
+        </is>
+      </c>
+      <c r="G637" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H637" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047583165-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="638">
       <c r="C638" t="inlineStr">
         <is>
@@ -10928,6 +11676,23 @@
         </is>
       </c>
     </row>
+    <row r="659">
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>1700004362957</t>
+        </is>
+      </c>
+      <c r="G659" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H659" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047585906-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="660">
       <c r="C660" t="inlineStr">
         <is>
@@ -10962,6 +11727,40 @@
         </is>
       </c>
     </row>
+    <row r="662">
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>1700011023730</t>
+        </is>
+      </c>
+      <c r="G662" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H662" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047586224-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>1700012269828</t>
+        </is>
+      </c>
+      <c r="G663" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H663" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047586347-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="664">
       <c r="C664" t="inlineStr">
         <is>
@@ -11030,6 +11829,23 @@
         </is>
       </c>
     </row>
+    <row r="668">
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>1700017091346</t>
+        </is>
+      </c>
+      <c r="G668" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H668" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047587229-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="669">
       <c r="C669" t="inlineStr">
         <is>
@@ -11081,6 +11897,23 @@
         </is>
       </c>
     </row>
+    <row r="672">
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>1700021773016</t>
+        </is>
+      </c>
+      <c r="G672" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H672" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047588469-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="673">
       <c r="C673" t="inlineStr">
         <is>
@@ -11115,6 +11948,23 @@
         </is>
       </c>
     </row>
+    <row r="675">
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>1700023584718</t>
+        </is>
+      </c>
+      <c r="G675" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H675" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047589214-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="676">
       <c r="C676" t="inlineStr">
         <is>
@@ -11506,6 +12356,23 @@
         </is>
       </c>
     </row>
+    <row r="699">
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>1700030337286</t>
+        </is>
+      </c>
+      <c r="G699" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H699" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047594989-C1 has dropped the video KYC. Ask the client to complete it by using this link http://www.axisbank.com/vkyc.</t>
+        </is>
+      </c>
+    </row>
     <row r="700">
       <c r="C700" t="inlineStr">
         <is>
@@ -11744,6 +12611,23 @@
         </is>
       </c>
     </row>
+    <row r="714">
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>1700033368784</t>
+        </is>
+      </c>
+      <c r="G714" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H714" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047597873-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="715">
       <c r="C715" t="inlineStr">
         <is>
@@ -12237,6 +13121,40 @@
         </is>
       </c>
     </row>
+    <row r="744">
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>1700047221224</t>
+        </is>
+      </c>
+      <c r="G744" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H744" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047608357-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>1700047077360</t>
+        </is>
+      </c>
+      <c r="G745" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H745" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047608542-C1 has dropped the video KYC. Ask the client to complete it by using this link http://www.axisbank.com/vkyc.</t>
+        </is>
+      </c>
+    </row>
     <row r="746">
       <c r="C746" t="inlineStr">
         <is>
@@ -12254,6 +13172,40 @@
         </is>
       </c>
     </row>
+    <row r="747">
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>1700047390202</t>
+        </is>
+      </c>
+      <c r="G747" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H747" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047608742-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>1700046786938</t>
+        </is>
+      </c>
+      <c r="G748" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H748" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047608949-C1 has dropped the video KYC. Ask the client to complete it by using this link http://www.axisbank.com/vkyc.</t>
+        </is>
+      </c>
+    </row>
     <row r="749">
       <c r="C749" t="inlineStr">
         <is>
@@ -12288,6 +13240,23 @@
         </is>
       </c>
     </row>
+    <row r="751">
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>1700047475333</t>
+        </is>
+      </c>
+      <c r="G751" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H751" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047609188-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="752">
       <c r="C752" t="inlineStr">
         <is>
@@ -12373,6 +13342,23 @@
         </is>
       </c>
     </row>
+    <row r="757">
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>1700050430930</t>
+        </is>
+      </c>
+      <c r="G757" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H757" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047610838-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="758">
       <c r="C758" t="inlineStr">
         <is>
@@ -12441,6 +13427,57 @@
         </is>
       </c>
     </row>
+    <row r="762">
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>1700052778053</t>
+        </is>
+      </c>
+      <c r="G762" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H762" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047612480-C1 has dropped the video KYC. Ask the client to complete it by using this link http://www.axisbank.com/vkyc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>1700053279040</t>
+        </is>
+      </c>
+      <c r="G763" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H763" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047612942-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>1700054383383</t>
+        </is>
+      </c>
+      <c r="G764" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H764" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047613324-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="765">
       <c r="C765" t="inlineStr">
         <is>
@@ -12492,6 +13529,23 @@
         </is>
       </c>
     </row>
+    <row r="768">
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>1700055226578</t>
+        </is>
+      </c>
+      <c r="G768" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H768" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047613803-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="769">
       <c r="C769" t="inlineStr">
         <is>
@@ -12509,6 +13563,23 @@
         </is>
       </c>
     </row>
+    <row r="770">
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>1700055981019</t>
+        </is>
+      </c>
+      <c r="G770" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H770" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047614198-C1 has dropped the video KYC. Ask the client to complete it by using this link http://www.axisbank.com/vkyc.</t>
+        </is>
+      </c>
+    </row>
     <row r="771">
       <c r="C771" t="inlineStr">
         <is>
@@ -12628,6 +13699,23 @@
         </is>
       </c>
     </row>
+    <row r="778">
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>1700059057020</t>
+        </is>
+      </c>
+      <c r="G778" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H778" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047615804-C1 has finished the video KYC. The client has to wait the final decision of the bank.</t>
+        </is>
+      </c>
+    </row>
     <row r="779">
       <c r="C779" t="inlineStr">
         <is>
@@ -12781,6 +13869,23 @@
         </is>
       </c>
     </row>
+    <row r="788">
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>1700071471921</t>
+        </is>
+      </c>
+      <c r="G788" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H788" t="inlineStr">
+        <is>
+          <t>The client with application number C1-00000047620023-C1 has dropped the video KYC. Ask the client to complete it by using this link http://www.axisbank.com/vkyc.</t>
+        </is>
+      </c>
+    </row>
     <row r="789">
       <c r="C789" t="inlineStr">
         <is>
@@ -12832,6 +13937,23 @@
         </is>
       </c>
     </row>
+    <row r="792">
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>1700075731208</t>
+        </is>
+      </c>
+      <c r="G792" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H792" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047620894-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
     <row r="793">
       <c r="C793" t="inlineStr">
         <is>
@@ -12846,6 +13968,74 @@
       <c r="H793" t="inlineStr">
         <is>
           <t>The customer with application number C1-00000047621310-C1 was rejected due to 0500 - Dip Reject.</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>1700088796026</t>
+        </is>
+      </c>
+      <c r="G794" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H794" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047621712-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>1700099002090</t>
+        </is>
+      </c>
+      <c r="G795" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H795" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047622203-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>1700103656960</t>
+        </is>
+      </c>
+      <c r="G796" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H796" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047622837-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>1700106553845</t>
+        </is>
+      </c>
+      <c r="G797" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H797" t="inlineStr">
+        <is>
+          <t>The client’s application is C1-00000047623622-C1. The Risk Team of the Bank is checking the profile, so your client has to wait.</t>
         </is>
       </c>
     </row>

</xml_diff>